<commit_message>
penambahan dataset m4 perbaikan struktur csv
</commit_message>
<xml_diff>
--- a/dataset/cacar-air-hungaria.xlsx
+++ b/dataset/cacar-air-hungaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\S2\Thesis\loss-function-comparison\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32368A8A-5CFF-4396-B5E8-48BEDC7D5BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D56F7-0287-4DAC-860B-1F0029B8D748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19000D87-57E7-4F1B-88AE-BA8A2A57D4C4}"/>
   </bookViews>
@@ -26,9 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Date</t>
-  </si>
   <si>
     <t>BUDAPEST</t>
   </si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>ZALA</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E026E6-A3E7-42D6-AD45-7A2E6692C911}">
   <dimension ref="A1:U523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,67 +962,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>